<commit_message>
getting the adv demo model ready for storage modeling examples
</commit_message>
<xml_diff>
--- a/Sets-DemoAdv.xlsx
+++ b/Sets-DemoAdv.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\NewVEDA\Veda_models\Demo_models\DemoS_Adv\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VEDA\VEDA_Models\Demo_Adv_Veda\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62CD74D9-999E-4507-AA87-6D72FB1732F7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A41952A4-E7C8-41F3-8532-3A81DA33C7EE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{91160169-4669-41EB-968B-C98B54EC51CB}"/>
+    <workbookView xWindow="7500" yWindow="1335" windowWidth="18135" windowHeight="11025" xr2:uid="{91160169-4669-41EB-968B-C98B54EC51CB}"/>
   </bookViews>
   <sheets>
     <sheet name="VEDA_Sets-Comm" sheetId="2" r:id="rId1"/>
@@ -748,7 +748,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB068F12-506D-4B74-BF24-03EBDA23C84D}">
   <dimension ref="A1:H9"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -925,8 +925,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71754C8A-E599-4286-919F-11B5789CC171}">
   <dimension ref="A1:J32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
after chat with Antti
</commit_message>
<xml_diff>
--- a/Sets-DemoAdv.xlsx
+++ b/Sets-DemoAdv.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VEDA\VEDA_Models\Demo_Adv_Veda\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A41952A4-E7C8-41F3-8532-3A81DA33C7EE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8419B1F9-AFB5-41B3-B80B-114ECA99C4D7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7500" yWindow="1335" windowWidth="18135" windowHeight="11025" xr2:uid="{91160169-4669-41EB-968B-C98B54EC51CB}"/>
+    <workbookView xWindow="8685" yWindow="1410" windowWidth="16170" windowHeight="14190" xr2:uid="{91160169-4669-41EB-968B-C98B54EC51CB}"/>
   </bookViews>
   <sheets>
     <sheet name="VEDA_Sets-Comm" sheetId="2" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="124">
   <si>
     <t>~TFM_Psets</t>
   </si>
@@ -118,9 +118,6 @@
     <t>ELECOA</t>
   </si>
   <si>
-    <t>ELE,STG</t>
-  </si>
-  <si>
     <t>ELC</t>
   </si>
   <si>
@@ -395,6 +392,18 @@
   </si>
   <si>
     <t>Other</t>
+  </si>
+  <si>
+    <t>ELE,STG,NST</t>
+  </si>
+  <si>
+    <t>*siftelc*</t>
+  </si>
+  <si>
+    <t>*pondage*,*large reservoir*</t>
+  </si>
+  <si>
+    <t>Or</t>
   </si>
 </sst>
 </file>
@@ -762,18 +771,18 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B2" t="s">
         <v>72</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>73</v>
-      </c>
-      <c r="C2" t="s">
-        <v>74</v>
       </c>
       <c r="D2" t="s">
         <v>6</v>
@@ -793,16 +802,16 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
+        <v>74</v>
+      </c>
+      <c r="C3" t="s">
         <v>75</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>76</v>
       </c>
-      <c r="D3" t="s">
-        <v>77</v>
-      </c>
       <c r="E3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F3" t="s">
         <v>12</v>
@@ -813,13 +822,13 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F4" t="s">
         <v>12</v>
@@ -830,16 +839,16 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F5" t="s">
         <v>12</v>
@@ -850,13 +859,13 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E6" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F6" t="s">
         <v>12</v>
@@ -867,13 +876,13 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D7" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E7" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F7" t="s">
         <v>12</v>
@@ -884,13 +893,13 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
+        <v>81</v>
+      </c>
+      <c r="D8" t="s">
         <v>82</v>
       </c>
-      <c r="D8" t="s">
-        <v>83</v>
-      </c>
       <c r="E8" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F8" t="s">
         <v>12</v>
@@ -901,13 +910,13 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C9" t="s">
+        <v>83</v>
+      </c>
+      <c r="D9" t="s">
         <v>84</v>
       </c>
-      <c r="D9" t="s">
-        <v>85</v>
-      </c>
       <c r="E9" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F9" t="s">
         <v>12</v>
@@ -976,16 +985,16 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F3" t="s">
         <v>11</v>
       </c>
       <c r="G3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H3" t="s">
         <v>12</v>
@@ -993,16 +1002,16 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F4" t="s">
         <v>13</v>
       </c>
       <c r="G4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H4" t="s">
         <v>12</v>
@@ -1013,13 +1022,13 @@
         <v>23</v>
       </c>
       <c r="E5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F5" t="s">
         <v>14</v>
       </c>
       <c r="G5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H5" t="s">
         <v>12</v>
@@ -1027,16 +1036,16 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F6" t="s">
         <v>15</v>
       </c>
       <c r="G6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H6" t="s">
         <v>12</v>
@@ -1044,16 +1053,16 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F7" t="s">
         <v>16</v>
       </c>
       <c r="G7" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="H7" t="s">
         <v>12</v>
@@ -1061,16 +1070,16 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E8" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F8" t="s">
         <v>17</v>
       </c>
       <c r="G8" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="H8" t="s">
         <v>12</v>
@@ -1087,7 +1096,7 @@
         <v>20</v>
       </c>
       <c r="G9" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H9" t="s">
         <v>12</v>
@@ -1101,7 +1110,7 @@
         <v>22</v>
       </c>
       <c r="G10" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="H10" t="s">
         <v>12</v>
@@ -1118,7 +1127,7 @@
         <v>25</v>
       </c>
       <c r="G11" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="H11" t="s">
         <v>12</v>
@@ -1135,7 +1144,7 @@
         <v>27</v>
       </c>
       <c r="G12" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="H12" t="s">
         <v>12</v>
@@ -1143,19 +1152,28 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>120</v>
+      </c>
+      <c r="B13" t="s">
+        <v>121</v>
+      </c>
+      <c r="C13" t="s">
+        <v>122</v>
+      </c>
+      <c r="D13" t="s">
         <v>28</v>
       </c>
-      <c r="D13" t="s">
+      <c r="F13" t="s">
         <v>29</v>
       </c>
-      <c r="F13" t="s">
-        <v>30</v>
-      </c>
       <c r="G13" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="H13" t="s">
-        <v>12</v>
+        <v>123</v>
+      </c>
+      <c r="I13" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
@@ -1163,13 +1181,13 @@
         <v>23</v>
       </c>
       <c r="D14" t="s">
+        <v>30</v>
+      </c>
+      <c r="F14" t="s">
         <v>31</v>
       </c>
-      <c r="F14" t="s">
-        <v>32</v>
-      </c>
       <c r="G14" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="H14" t="s">
         <v>12</v>
@@ -1180,13 +1198,13 @@
         <v>23</v>
       </c>
       <c r="D15" t="s">
+        <v>32</v>
+      </c>
+      <c r="F15" t="s">
         <v>33</v>
       </c>
-      <c r="F15" t="s">
-        <v>34</v>
-      </c>
       <c r="G15" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H15" t="s">
         <v>12</v>
@@ -1197,13 +1215,13 @@
         <v>23</v>
       </c>
       <c r="D16" t="s">
+        <v>34</v>
+      </c>
+      <c r="F16" t="s">
         <v>35</v>
       </c>
-      <c r="F16" t="s">
-        <v>36</v>
-      </c>
       <c r="G16" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H16" t="s">
         <v>12</v>
@@ -1214,13 +1232,13 @@
         <v>23</v>
       </c>
       <c r="D17" t="s">
+        <v>36</v>
+      </c>
+      <c r="F17" t="s">
         <v>37</v>
       </c>
-      <c r="F17" t="s">
-        <v>38</v>
-      </c>
       <c r="G17" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H17" t="s">
         <v>12</v>
@@ -1231,13 +1249,13 @@
         <v>23</v>
       </c>
       <c r="D18" t="s">
+        <v>38</v>
+      </c>
+      <c r="F18" t="s">
         <v>39</v>
       </c>
-      <c r="F18" t="s">
-        <v>40</v>
-      </c>
       <c r="G18" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="H18" t="s">
         <v>12</v>
@@ -1248,13 +1266,13 @@
         <v>23</v>
       </c>
       <c r="D19" t="s">
+        <v>40</v>
+      </c>
+      <c r="F19" t="s">
         <v>41</v>
       </c>
-      <c r="F19" t="s">
-        <v>42</v>
-      </c>
       <c r="G19" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="H19" t="s">
         <v>12</v>
@@ -1262,13 +1280,13 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
+        <v>42</v>
+      </c>
+      <c r="F20" t="s">
         <v>43</v>
       </c>
-      <c r="F20" t="s">
-        <v>44</v>
-      </c>
       <c r="G20" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H20" t="s">
         <v>12</v>
@@ -1276,19 +1294,19 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
+        <v>44</v>
+      </c>
+      <c r="B21" t="s">
+        <v>55</v>
+      </c>
+      <c r="E21" t="s">
         <v>45</v>
       </c>
-      <c r="B21" t="s">
-        <v>56</v>
-      </c>
-      <c r="E21" t="s">
+      <c r="F21" t="s">
         <v>46</v>
       </c>
-      <c r="F21" t="s">
-        <v>47</v>
-      </c>
       <c r="G21" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H21" t="s">
         <v>12</v>
@@ -1296,19 +1314,19 @@
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B22" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E22" t="s">
+        <v>47</v>
+      </c>
+      <c r="F22" t="s">
         <v>48</v>
       </c>
-      <c r="F22" t="s">
-        <v>49</v>
-      </c>
       <c r="G22" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H22" t="s">
         <v>12</v>
@@ -1316,19 +1334,19 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B23" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E23" t="s">
+        <v>49</v>
+      </c>
+      <c r="F23" t="s">
         <v>50</v>
       </c>
-      <c r="F23" t="s">
-        <v>51</v>
-      </c>
       <c r="G23" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H23" t="s">
         <v>12</v>
@@ -1336,19 +1354,19 @@
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B24" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E24" t="s">
+        <v>51</v>
+      </c>
+      <c r="F24" t="s">
         <v>52</v>
       </c>
-      <c r="F24" t="s">
-        <v>53</v>
-      </c>
       <c r="G24" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="H24" t="s">
         <v>12</v>
@@ -1356,19 +1374,19 @@
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B25" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E25" t="s">
+        <v>53</v>
+      </c>
+      <c r="F25" t="s">
         <v>54</v>
       </c>
-      <c r="F25" t="s">
-        <v>55</v>
-      </c>
       <c r="G25" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="H25" t="s">
         <v>12</v>
@@ -1376,13 +1394,13 @@
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
+        <v>55</v>
+      </c>
+      <c r="F26" t="s">
         <v>56</v>
       </c>
-      <c r="F26" t="s">
-        <v>57</v>
-      </c>
       <c r="G26" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="H26" t="s">
         <v>12</v>
@@ -1390,13 +1408,13 @@
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
+        <v>57</v>
+      </c>
+      <c r="F27" t="s">
         <v>58</v>
       </c>
-      <c r="F27" t="s">
-        <v>59</v>
-      </c>
       <c r="G27" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="H27" t="s">
         <v>12</v>
@@ -1407,13 +1425,13 @@
         <v>18</v>
       </c>
       <c r="B28" t="s">
+        <v>59</v>
+      </c>
+      <c r="F28" t="s">
         <v>60</v>
       </c>
-      <c r="F28" t="s">
-        <v>61</v>
-      </c>
       <c r="G28" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="H28" t="s">
         <v>12</v>
@@ -1424,13 +1442,13 @@
         <v>23</v>
       </c>
       <c r="D29" t="s">
+        <v>61</v>
+      </c>
+      <c r="F29" t="s">
         <v>62</v>
       </c>
-      <c r="F29" t="s">
-        <v>63</v>
-      </c>
       <c r="G29" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="H29" t="s">
         <v>12</v>
@@ -1441,13 +1459,13 @@
         <v>23</v>
       </c>
       <c r="D30" t="s">
+        <v>63</v>
+      </c>
+      <c r="F30" t="s">
         <v>64</v>
       </c>
-      <c r="F30" t="s">
-        <v>65</v>
-      </c>
       <c r="G30" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H30" t="s">
         <v>12</v>
@@ -1455,16 +1473,16 @@
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
+        <v>65</v>
+      </c>
+      <c r="B31" t="s">
         <v>66</v>
       </c>
-      <c r="B31" t="s">
+      <c r="F31" t="s">
         <v>67</v>
       </c>
-      <c r="F31" t="s">
-        <v>68</v>
-      </c>
       <c r="G31" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="H31" t="s">
         <v>12</v>
@@ -1475,13 +1493,13 @@
         <v>23</v>
       </c>
       <c r="D32" t="s">
+        <v>68</v>
+      </c>
+      <c r="F32" t="s">
         <v>69</v>
       </c>
-      <c r="F32" t="s">
-        <v>70</v>
-      </c>
       <c r="G32" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H32" t="s">
         <v>12</v>

</xml_diff>

<commit_message>
testing V1G and V2G
</commit_message>
<xml_diff>
--- a/Sets-DemoAdv.xlsx
+++ b/Sets-DemoAdv.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VEDA\VEDA_Models\Demo_Adv_Veda\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VEDA\Veda\Veda_models\Demo_Adv_Veda\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33708918-884F-46DA-B522-B4EF43C1BF8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8441E0A-6C41-45E9-B4D0-CAC8625EC9E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{91160169-4669-41EB-968B-C98B54EC51CB}"/>
+    <workbookView xWindow="3420" yWindow="3420" windowWidth="21600" windowHeight="12735" activeTab="2" xr2:uid="{91160169-4669-41EB-968B-C98B54EC51CB}"/>
   </bookViews>
   <sheets>
     <sheet name="SetsEditor- Comm" sheetId="3" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="147">
   <si>
     <t>~TFM_Psets</t>
   </si>
@@ -465,6 +465,15 @@
   </si>
   <si>
     <t>SecFueIND</t>
+  </si>
+  <si>
+    <t>TRAELC</t>
+  </si>
+  <si>
+    <t>V2G</t>
+  </si>
+  <si>
+    <t>vehicle2Grid</t>
   </si>
 </sst>
 </file>
@@ -818,7 +827,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3385AAE9-23B6-448E-B7EC-32078070A32D}">
   <dimension ref="A1:I7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
@@ -1174,10 +1183,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71754C8A-E599-4286-919F-11B5789CC171}">
-  <dimension ref="A1:J32"/>
+  <dimension ref="A1:J33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A28" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G34" sqref="G34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1747,6 +1757,20 @@
         <v>12</v>
       </c>
     </row>
+    <row r="33" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D33" t="s">
+        <v>144</v>
+      </c>
+      <c r="E33" t="s">
+        <v>28</v>
+      </c>
+      <c r="F33" t="s">
+        <v>145</v>
+      </c>
+      <c r="G33" t="s">
+        <v>146</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
creating new definitions for process/commodity map
</commit_message>
<xml_diff>
--- a/Sets-DemoAdv.xlsx
+++ b/Sets-DemoAdv.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VEDA\Veda\Veda_models\Demo_Adv_Veda\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8441E0A-6C41-45E9-B4D0-CAC8625EC9E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C3A3475-2122-438B-B63D-2863B28F08D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3420" yWindow="3420" windowWidth="21600" windowHeight="12735" activeTab="2" xr2:uid="{91160169-4669-41EB-968B-C98B54EC51CB}"/>
+    <workbookView xWindow="2340" yWindow="2340" windowWidth="21600" windowHeight="12735" activeTab="1" xr2:uid="{91160169-4669-41EB-968B-C98B54EC51CB}"/>
   </bookViews>
   <sheets>
     <sheet name="SetsEditor- Comm" sheetId="3" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="150">
   <si>
     <t>~TFM_Psets</t>
   </si>
@@ -278,9 +278,6 @@
     <t>*OIL*,*DSL*,*LPG*,*GSL*,*KER*,*OPP*,*HFO*,*NAP*</t>
   </si>
   <si>
-    <t>*BIO*,*SOL*,*WIN*,*RNW*,*HYD*,-*SOLID*,-ELCRNW,-RNW</t>
-  </si>
-  <si>
     <t>NRG_RNW</t>
   </si>
   <si>
@@ -474,6 +471,18 @@
   </si>
   <si>
     <t>vehicle2Grid</t>
+  </si>
+  <si>
+    <t>c_Pos_AndOr</t>
+  </si>
+  <si>
+    <t>c_Neg_AndOr</t>
+  </si>
+  <si>
+    <t>*BIO*</t>
+  </si>
+  <si>
+    <t>*SOL*,*WIN*,*RNW*,*HYD*,-*SOLID*,-ELCRNW,-RNW</t>
   </si>
 </sst>
 </file>
@@ -835,166 +844,166 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>124</v>
+      </c>
+      <c r="B2" t="s">
         <v>125</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>126</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>127</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>128</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>129</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>130</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>131</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>132</v>
-      </c>
-      <c r="I2" t="s">
-        <v>133</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>133</v>
+      </c>
+      <c r="B3" t="s">
+        <v>99</v>
+      </c>
+      <c r="C3" t="s">
         <v>134</v>
-      </c>
-      <c r="B3" t="s">
-        <v>100</v>
-      </c>
-      <c r="C3" t="s">
-        <v>135</v>
       </c>
       <c r="D3" t="s">
         <v>45</v>
       </c>
       <c r="F3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="H3" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="I3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>136</v>
+      </c>
+      <c r="B4" t="s">
+        <v>103</v>
+      </c>
+      <c r="C4" t="s">
+        <v>134</v>
+      </c>
+      <c r="D4" t="s">
         <v>137</v>
       </c>
-      <c r="B4" t="s">
-        <v>104</v>
-      </c>
-      <c r="C4" t="s">
-        <v>135</v>
-      </c>
-      <c r="D4" t="s">
-        <v>138</v>
-      </c>
       <c r="F4" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G4" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="H4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="I4" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B5" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C5" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D5" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F5" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G5" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="H5" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="I5" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>139</v>
+      </c>
+      <c r="B6" t="s">
+        <v>100</v>
+      </c>
+      <c r="C6" t="s">
+        <v>134</v>
+      </c>
+      <c r="D6" t="s">
         <v>140</v>
       </c>
-      <c r="B6" t="s">
-        <v>101</v>
-      </c>
-      <c r="C6" t="s">
-        <v>135</v>
-      </c>
-      <c r="D6" t="s">
-        <v>141</v>
-      </c>
       <c r="F6" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G6" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="H6" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="I6" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B7" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C7" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D7" t="s">
         <v>49</v>
       </c>
       <c r="F7" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G7" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="H7" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="I7" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
   </sheetData>
@@ -1006,8 +1015,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB068F12-506D-4B74-BF24-03EBDA23C84D}">
   <dimension ref="A1:H9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1042,10 +1051,10 @@
         <v>7</v>
       </c>
       <c r="F2" t="s">
-        <v>8</v>
+        <v>146</v>
       </c>
       <c r="G2" t="s">
-        <v>9</v>
+        <v>147</v>
       </c>
       <c r="H2" t="s">
         <v>10</v>
@@ -1062,7 +1071,7 @@
         <v>76</v>
       </c>
       <c r="E3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F3" t="s">
         <v>12</v>
@@ -1072,6 +1081,9 @@
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>134</v>
+      </c>
       <c r="B4" t="s">
         <v>30</v>
       </c>
@@ -1079,18 +1091,18 @@
         <v>77</v>
       </c>
       <c r="E4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F4" t="s">
-        <v>12</v>
+        <v>135</v>
       </c>
       <c r="G4" t="s">
-        <v>12</v>
+        <v>135</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B5" t="s">
         <v>66</v>
@@ -1099,7 +1111,7 @@
         <v>78</v>
       </c>
       <c r="E5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F5" t="s">
         <v>12</v>
@@ -1116,7 +1128,7 @@
         <v>79</v>
       </c>
       <c r="E6" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F6" t="s">
         <v>12</v>
@@ -1126,54 +1138,66 @@
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>134</v>
+      </c>
       <c r="B7" t="s">
         <v>80</v>
       </c>
       <c r="D7" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E7" t="s">
+        <v>89</v>
+      </c>
+      <c r="F7" t="s">
+        <v>135</v>
+      </c>
+      <c r="G7" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>134</v>
+      </c>
+      <c r="B8" t="s">
+        <v>149</v>
+      </c>
+      <c r="D8" t="s">
+        <v>81</v>
+      </c>
+      <c r="E8" t="s">
         <v>90</v>
       </c>
-      <c r="F7" t="s">
-        <v>12</v>
-      </c>
-      <c r="G7" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
-        <v>81</v>
-      </c>
-      <c r="D8" t="s">
+      <c r="F8" t="s">
+        <v>135</v>
+      </c>
+      <c r="G8" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>134</v>
+      </c>
+      <c r="B9" t="s">
+        <v>148</v>
+      </c>
+      <c r="C9" t="s">
         <v>82</v>
       </c>
-      <c r="E8" t="s">
+      <c r="D9" t="s">
+        <v>83</v>
+      </c>
+      <c r="E9" t="s">
         <v>91</v>
       </c>
-      <c r="F8" t="s">
-        <v>12</v>
-      </c>
-      <c r="G8" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C9" t="s">
-        <v>83</v>
-      </c>
-      <c r="D9" t="s">
-        <v>84</v>
-      </c>
-      <c r="E9" t="s">
-        <v>92</v>
-      </c>
       <c r="F9" t="s">
-        <v>12</v>
+        <v>122</v>
       </c>
       <c r="G9" t="s">
-        <v>12</v>
+        <v>135</v>
       </c>
     </row>
   </sheetData>
@@ -1185,7 +1209,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71754C8A-E599-4286-919F-11B5789CC171}">
   <dimension ref="A1:J33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A28" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="G34" sqref="G34"/>
     </sheetView>
@@ -1237,16 +1261,16 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F3" t="s">
         <v>11</v>
       </c>
       <c r="G3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="H3" t="s">
         <v>12</v>
@@ -1254,16 +1278,16 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F4" t="s">
         <v>13</v>
       </c>
       <c r="G4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H4" t="s">
         <v>12</v>
@@ -1280,7 +1304,7 @@
         <v>14</v>
       </c>
       <c r="G5" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H5" t="s">
         <v>12</v>
@@ -1288,16 +1312,16 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E6" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F6" t="s">
         <v>15</v>
       </c>
       <c r="G6" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H6" t="s">
         <v>12</v>
@@ -1305,16 +1329,16 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F7" t="s">
         <v>16</v>
       </c>
       <c r="G7" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H7" t="s">
         <v>12</v>
@@ -1322,16 +1346,16 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E8" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F8" t="s">
         <v>17</v>
       </c>
       <c r="G8" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="H8" t="s">
         <v>12</v>
@@ -1348,7 +1372,7 @@
         <v>20</v>
       </c>
       <c r="G9" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="H9" t="s">
         <v>12</v>
@@ -1362,7 +1386,7 @@
         <v>22</v>
       </c>
       <c r="G10" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H10" t="s">
         <v>12</v>
@@ -1379,7 +1403,7 @@
         <v>25</v>
       </c>
       <c r="G11" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="H11" t="s">
         <v>12</v>
@@ -1396,7 +1420,7 @@
         <v>27</v>
       </c>
       <c r="G12" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="H12" t="s">
         <v>12</v>
@@ -1404,13 +1428,13 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>119</v>
+      </c>
+      <c r="B13" t="s">
         <v>120</v>
       </c>
-      <c r="B13" t="s">
+      <c r="C13" t="s">
         <v>121</v>
-      </c>
-      <c r="C13" t="s">
-        <v>122</v>
       </c>
       <c r="D13" t="s">
         <v>28</v>
@@ -1419,13 +1443,13 @@
         <v>29</v>
       </c>
       <c r="G13" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="H13" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="I13" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
@@ -1439,7 +1463,7 @@
         <v>31</v>
       </c>
       <c r="G14" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H14" t="s">
         <v>12</v>
@@ -1456,7 +1480,7 @@
         <v>33</v>
       </c>
       <c r="G15" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="H15" t="s">
         <v>12</v>
@@ -1473,7 +1497,7 @@
         <v>35</v>
       </c>
       <c r="G16" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H16" t="s">
         <v>12</v>
@@ -1490,7 +1514,7 @@
         <v>37</v>
       </c>
       <c r="G17" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H17" t="s">
         <v>12</v>
@@ -1507,7 +1531,7 @@
         <v>39</v>
       </c>
       <c r="G18" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H18" t="s">
         <v>12</v>
@@ -1524,7 +1548,7 @@
         <v>41</v>
       </c>
       <c r="G19" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="H19" t="s">
         <v>12</v>
@@ -1538,7 +1562,7 @@
         <v>43</v>
       </c>
       <c r="G20" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="H20" t="s">
         <v>12</v>
@@ -1558,7 +1582,7 @@
         <v>46</v>
       </c>
       <c r="G21" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="H21" t="s">
         <v>12</v>
@@ -1578,7 +1602,7 @@
         <v>48</v>
       </c>
       <c r="G22" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H22" t="s">
         <v>12</v>
@@ -1598,7 +1622,7 @@
         <v>50</v>
       </c>
       <c r="G23" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H23" t="s">
         <v>12</v>
@@ -1618,7 +1642,7 @@
         <v>52</v>
       </c>
       <c r="G24" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H24" t="s">
         <v>12</v>
@@ -1638,7 +1662,7 @@
         <v>54</v>
       </c>
       <c r="G25" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="H25" t="s">
         <v>12</v>
@@ -1652,7 +1676,7 @@
         <v>56</v>
       </c>
       <c r="G26" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H26" t="s">
         <v>12</v>
@@ -1666,7 +1690,7 @@
         <v>58</v>
       </c>
       <c r="G27" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="H27" t="s">
         <v>12</v>
@@ -1683,7 +1707,7 @@
         <v>60</v>
       </c>
       <c r="G28" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="H28" t="s">
         <v>12</v>
@@ -1700,7 +1724,7 @@
         <v>62</v>
       </c>
       <c r="G29" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="H29" t="s">
         <v>12</v>
@@ -1717,7 +1741,7 @@
         <v>64</v>
       </c>
       <c r="G30" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H30" t="s">
         <v>12</v>
@@ -1734,7 +1758,7 @@
         <v>67</v>
       </c>
       <c r="G31" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="H31" t="s">
         <v>12</v>
@@ -1751,7 +1775,7 @@
         <v>69</v>
       </c>
       <c r="G32" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H32" t="s">
         <v>12</v>
@@ -1759,16 +1783,16 @@
     </row>
     <row r="33" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D33" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E33" t="s">
         <v>28</v>
       </c>
       <c r="F33" t="s">
+        <v>144</v>
+      </c>
+      <c r="G33" t="s">
         <v>145</v>
-      </c>
-      <c r="G33" t="s">
-        <v>146</v>
       </c>
     </row>
   </sheetData>

</xml_diff>